<commit_message>
Auditoria del mes de Abril
</commit_message>
<xml_diff>
--- a/qualtcom/Procesos/Calidad/Checklist_Auditoría-150430.xlsx
+++ b/qualtcom/Procesos/Calidad/Checklist_Auditoría-150430.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayra\qtp\qualtcom\Procesos\Calidad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\proyecto\qualtcom\Procesos\Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="119">
   <si>
     <t>DATOS GENERALES</t>
   </si>
@@ -87,6 +87,18 @@
   </si>
   <si>
     <t>NO APLICA</t>
+  </si>
+  <si>
+    <t>¿Se generó el catalogo de servicios?</t>
+  </si>
+  <si>
+    <t>¿Se definieron estrategias para el servicio?</t>
+  </si>
+  <si>
+    <t>¿Se generó la estimación anual?</t>
+  </si>
+  <si>
+    <t>¿Se genero los planes de apoyo?</t>
   </si>
   <si>
     <t>¿Se generó el compromiso acorde al plan estratégico?</t>
@@ -275,6 +287,15 @@
     <t>Ejecución</t>
   </si>
   <si>
+    <t>¿Se asigno un responsable?</t>
+  </si>
+  <si>
+    <t>¿Se resolvio el ticket?</t>
+  </si>
+  <si>
+    <t>¿Se cerro el ticket?</t>
+  </si>
+  <si>
     <t>Plan Estrategico</t>
   </si>
   <si>
@@ -284,10 +305,16 @@
     <t>Estimación</t>
   </si>
   <si>
+    <t>¿Se realizo la encuesta de satisfacción?</t>
+  </si>
+  <si>
     <t>Ante un cambio que afecte la Línea base ¿Se ha actualizado la misma y se identifica el cambio en la version de linea base?</t>
   </si>
   <si>
     <t xml:space="preserve">Ticket de servicio </t>
+  </si>
+  <si>
+    <t>Se asignarion todos los tickets?</t>
   </si>
   <si>
     <t>Todos los tickets cuentan con una descripcion?</t>
@@ -354,48 +381,6 @@
   </si>
   <si>
     <t>Se genero encuestas a partir del mes de abril</t>
-  </si>
-  <si>
-    <t>¿Se asignó un responsable por ticket?</t>
-  </si>
-  <si>
-    <t>¿Se resolvió el ticket en el tiempo especificado?</t>
-  </si>
-  <si>
-    <t>¿El ticket tiene asignada una fecha de compromiso?</t>
-  </si>
-  <si>
-    <t>¿Se cerró el ticket en la fecha especificada?</t>
-  </si>
-  <si>
-    <t>¿Se realizó la encuesta de satisfacción al cliente?</t>
-  </si>
-  <si>
-    <t>¿Se generó el catálogo de servicios al inicio de la planeación?</t>
-  </si>
-  <si>
-    <t>¿Se definieron estrategias para este servicio?</t>
-  </si>
-  <si>
-    <t>¿Se generó la estimación anual del proyecto al inicio de la planeación?</t>
-  </si>
-  <si>
-    <t>¿Se generó el plan de riesgos?</t>
-  </si>
-  <si>
-    <t>¿Se generó el plan de calidad?</t>
-  </si>
-  <si>
-    <t>¿Se generó el plan de medición?</t>
-  </si>
-  <si>
-    <t>¿Se generó el plan de configuración?</t>
-  </si>
-  <si>
-    <t>¿Se realizó por lo menos una vez al mes respaldo por equipo(Copia de Seguridad) ?</t>
-  </si>
-  <si>
-    <t>¿Se realizó por lo menos una vez al mes limpieza por equipo(Revisión por instalación, desfragmentación del disco duro, Liberación de espacion en disco duro, Ejecución de Antivirus) ?</t>
   </si>
 </sst>
 </file>
@@ -1239,7 +1224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -1279,7 +1264,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="49" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="D5" s="49"/>
       <c r="E5" s="49"/>
@@ -1290,7 +1275,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="D6" s="49"/>
       <c r="E6" s="49"/>
@@ -1301,7 +1286,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="D7" s="49"/>
       <c r="E7" s="49"/>
@@ -1312,7 +1297,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D8" s="49"/>
       <c r="E8" s="49"/>
@@ -1321,7 +1306,7 @@
     <row r="9" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="10" spans="1:6" ht="16.5" customHeight="1">
       <c r="B10" s="1" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
@@ -1349,25 +1334,25 @@
         <v>Planeación</v>
       </c>
       <c r="C13" s="9">
-        <f>COUNTA(Proceso!D3:D10)</f>
-        <v>8</v>
+        <f>COUNTA(Proceso!D3:D7)</f>
+        <v>5</v>
       </c>
       <c r="D13" s="10">
-        <f>COUNTIF((Proceso!D3:D10),"x")/(COUNTIF((Proceso!D3:D10),"x")+COUNTIF((Proceso!E3:E10),"x"))</f>
+        <f>COUNTIF((Proceso!D3:D7),"x")/(COUNTIF((Proceso!D3:D7),"x")+COUNTIF((Proceso!E3:E7),"x"))</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
       <c r="B14" s="8" t="str">
-        <f>Proceso!C12</f>
+        <f>Proceso!C9</f>
         <v>Ejecución</v>
       </c>
       <c r="C14" s="9">
-        <f>COUNTA(Proceso!D14:D19)</f>
-        <v>6</v>
+        <f>COUNTA(Proceso!D11:D15)</f>
+        <v>5</v>
       </c>
       <c r="D14" s="10">
-        <f>COUNTIF((Proceso!D14:D19),"x")/(COUNTIF((Proceso!D14:D19),"x")+COUNTIF((Proceso!E14:E19),"x"))</f>
+        <f>COUNTIF((Proceso!D11:D15),"x")/(COUNTIF((Proceso!D11:D15),"x")+COUNTIF((Proceso!E11:E15),"x"))</f>
         <v>1</v>
       </c>
     </row>
@@ -1415,7 +1400,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="10">
-        <f>COUNTIF((Proceso!D3:D10),"x")/(COUNTIF((Proceso!D3:D10),"x")+COUNTIF((Proceso!E3:E10),"x"))</f>
+        <f>COUNTIF((Proceso!D3:D7),"x")/(COUNTIF((Proceso!D3:D7),"x")+COUNTIF((Proceso!E3:E7),"x"))</f>
         <v>1</v>
       </c>
     </row>
@@ -1429,7 +1414,7 @@
         <v>6</v>
       </c>
       <c r="D20" s="10">
-        <f>COUNTIF((Proceso!D3:D10),"x")/(COUNTIF((Proceso!D3:D10),"x")+COUNTIF((Proceso!E3:E10),"x"))</f>
+        <f>COUNTIF((Proceso!D3:D7),"x")/(COUNTIF((Proceso!D3:D7),"x")+COUNTIF((Proceso!E3:E7),"x"))</f>
         <v>1</v>
       </c>
     </row>
@@ -1491,7 +1476,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="10">
-        <f>COUNTIF((Proceso!D18:D18),"x")/(COUNTIF((Proceso!D18:D18),"x")+COUNTIF((Proceso!E18:E18),"x"))</f>
+        <f>COUNTIF((Proceso!D14:D14),"x")/(COUNTIF((Proceso!D14:D14),"x")+COUNTIF((Proceso!E14:E14),"x"))</f>
         <v>1</v>
       </c>
     </row>
@@ -1554,11 +1539,11 @@
         <v>14</v>
       </c>
       <c r="C33" s="9">
-        <f>COUNTA(Funcional!D18:D21)</f>
+        <f>COUNTA(Funcional!D16:D19)</f>
         <v>0</v>
       </c>
       <c r="D33" s="10" t="e">
-        <f>COUNTIF((Funcional!D18:D21),"x")/(COUNTIF((Funcional!D18:D21),"x")+COUNTIF((Funcional!E18:E21),"x"))</f>
+        <f>COUNTIF((Funcional!D16:D19),"x")/(COUNTIF((Funcional!D16:D19),"x")+COUNTIF((Funcional!E16:E19),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1585,10 +1570,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ19"/>
+  <dimension ref="A1:AMJ15"/>
   <sheetViews>
     <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1603,10 +1588,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="14.45" customHeight="1">
       <c r="C1" s="50" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D1" s="52" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E1" s="53"/>
       <c r="F1" s="54"/>
@@ -1629,10 +1614,10 @@
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3" s="40" t="s">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="22"/>
@@ -1642,10 +1627,10 @@
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4" s="21" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E4" s="22"/>
       <c r="F4" s="22"/>
@@ -1655,10 +1640,10 @@
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5" s="21" t="s">
-        <v>117</v>
+        <v>23</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
@@ -1668,10 +1653,10 @@
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6" s="21" t="s">
-        <v>118</v>
+        <v>24</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
@@ -1681,84 +1666,78 @@
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7" s="21" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="22"/>
       <c r="G7" s="23"/>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8" s="21" t="s">
-        <v>120</v>
+    <row r="9" spans="1:7">
+      <c r="C9" s="50" t="s">
+        <v>86</v>
       </c>
-      <c r="D8" s="22" t="s">
-        <v>93</v>
+      <c r="D9" s="52" t="s">
+        <v>52</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10" s="21" t="s">
-        <v>21</v>
+      <c r="C10" s="51"/>
+      <c r="D10" s="20" t="s">
+        <v>18</v>
       </c>
-      <c r="D10" s="22" t="s">
-        <v>93</v>
+      <c r="E10" s="20" t="s">
+        <v>19</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23"/>
+      <c r="F10" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="19"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="C11" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="C12" s="50" t="s">
-        <v>82</v>
+      <c r="C12" s="21" t="s">
+        <v>87</v>
       </c>
-      <c r="D12" s="52" t="s">
-        <v>48</v>
+      <c r="D12" s="22" t="s">
+        <v>102</v>
       </c>
-      <c r="E12" s="53"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="18"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="C13" s="51"/>
-      <c r="D13" s="20" t="s">
-        <v>18</v>
+      <c r="C13" s="21" t="s">
+        <v>88</v>
       </c>
-      <c r="E13" s="20" t="s">
-        <v>19</v>
+      <c r="D13" s="22" t="s">
+        <v>102</v>
       </c>
-      <c r="F13" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="19"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="C14" s="40" t="s">
-        <v>96</v>
+      <c r="C14" s="21" t="s">
+        <v>89</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
@@ -1766,65 +1745,21 @@
     </row>
     <row r="15" spans="1:7">
       <c r="C15" s="21" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
       <c r="G15" s="23"/>
     </row>
-    <row r="16" spans="1:7">
-      <c r="C16" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="23"/>
-    </row>
-    <row r="17" spans="3:7">
-      <c r="C17" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="23"/>
-    </row>
-    <row r="18" spans="3:7">
-      <c r="C18" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="23"/>
-    </row>
-    <row r="19" spans="3:7">
-      <c r="C19" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="23"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:F1"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1834,10 +1769,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ41"/>
+  <dimension ref="A1:AMJ42"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A13" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1851,10 +1786,10 @@
   <sheetData>
     <row r="1" spans="2:1024">
       <c r="B1" s="58" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D1" s="53"/>
       <c r="E1" s="54"/>
@@ -1875,10 +1810,10 @@
     </row>
     <row r="3" spans="2:1024" customFormat="1">
       <c r="B3" s="21" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
@@ -2904,10 +2839,10 @@
     </row>
     <row r="4" spans="2:1024" customFormat="1">
       <c r="B4" s="21" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
@@ -3933,10 +3868,10 @@
     </row>
     <row r="5" spans="2:1024" customFormat="1">
       <c r="B5" s="21" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -4962,10 +4897,10 @@
     </row>
     <row r="6" spans="2:1024" customFormat="1">
       <c r="B6" s="21" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -5991,10 +5926,10 @@
     </row>
     <row r="7" spans="2:1024" customFormat="1">
       <c r="B7" s="21" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -7020,10 +6955,10 @@
     </row>
     <row r="8" spans="2:1024" customFormat="1">
       <c r="B8" s="21" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -8049,10 +7984,10 @@
     </row>
     <row r="9" spans="2:1024" customFormat="1">
       <c r="B9" s="21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
@@ -9078,10 +9013,10 @@
     </row>
     <row r="10" spans="2:1024" customFormat="1">
       <c r="B10" s="21" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -10107,10 +10042,10 @@
     </row>
     <row r="11" spans="2:1024" customFormat="1">
       <c r="B11" s="21" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
@@ -11136,10 +11071,10 @@
     </row>
     <row r="12" spans="2:1024" customFormat="1">
       <c r="B12" s="21" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -12165,10 +12100,10 @@
     </row>
     <row r="13" spans="2:1024" customFormat="1">
       <c r="B13" s="21" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -13194,10 +13129,10 @@
     </row>
     <row r="14" spans="2:1024" customFormat="1">
       <c r="B14" s="21" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -15248,10 +15183,10 @@
     </row>
     <row r="16" spans="2:1024" customFormat="1">
       <c r="B16" s="50" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="C16" s="52" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D16" s="53"/>
       <c r="E16" s="54"/>
@@ -17308,10 +17243,10 @@
     </row>
     <row r="18" spans="2:1024" customFormat="1">
       <c r="B18" s="21" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -18337,10 +18272,10 @@
     </row>
     <row r="19" spans="2:1024" customFormat="1">
       <c r="B19" s="21" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -19366,10 +19301,10 @@
     </row>
     <row r="20" spans="2:1024" customFormat="1">
       <c r="B20" s="21" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -20395,10 +20330,10 @@
     </row>
     <row r="21" spans="2:1024" customFormat="1">
       <c r="B21" s="21" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
@@ -21424,10 +21359,10 @@
     </row>
     <row r="22" spans="2:1024" customFormat="1">
       <c r="B22" s="21" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -22453,10 +22388,10 @@
     </row>
     <row r="23" spans="2:1024" customFormat="1">
       <c r="B23" s="21" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -23482,10 +23417,10 @@
     </row>
     <row r="24" spans="2:1024" customFormat="1">
       <c r="B24" s="21" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -25536,10 +25471,10 @@
     </row>
     <row r="26" spans="2:1024" customFormat="1">
       <c r="B26" s="50" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C26" s="52" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D26" s="53"/>
       <c r="E26" s="54"/>
@@ -27596,10 +27531,10 @@
     </row>
     <row r="28" spans="2:1024" customFormat="1">
       <c r="B28" s="16" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C28" s="43" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="43"/>
@@ -28625,10 +28560,10 @@
     </row>
     <row r="29" spans="2:1024" customFormat="1">
       <c r="B29" s="24" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C29" s="43" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="43"/>
@@ -29654,10 +29589,10 @@
     </row>
     <row r="30" spans="2:1024" customFormat="1">
       <c r="B30" s="24" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C30" s="43" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="43"/>
@@ -30683,10 +30618,10 @@
     </row>
     <row r="31" spans="2:1024" customFormat="1">
       <c r="B31" s="16" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C31" s="43" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="43"/>
@@ -31712,10 +31647,10 @@
     </row>
     <row r="32" spans="2:1024" customFormat="1">
       <c r="B32" s="16" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C32" s="43" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="43"/>
@@ -32739,30 +32674,1047 @@
       <c r="AMI32" s="17"/>
       <c r="AMJ32" s="17"/>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33"/>
+    <row r="33" spans="2:1024" customFormat="1">
       <c r="B33" s="16" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C33" s="43" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="43"/>
       <c r="F33" s="16"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="17"/>
+      <c r="U33" s="17"/>
+      <c r="V33" s="17"/>
+      <c r="W33" s="17"/>
+      <c r="X33" s="17"/>
+      <c r="Y33" s="17"/>
+      <c r="Z33" s="17"/>
+      <c r="AA33" s="17"/>
+      <c r="AB33" s="17"/>
+      <c r="AC33" s="17"/>
+      <c r="AD33" s="17"/>
+      <c r="AE33" s="17"/>
+      <c r="AF33" s="17"/>
+      <c r="AG33" s="17"/>
+      <c r="AH33" s="17"/>
+      <c r="AI33" s="17"/>
+      <c r="AJ33" s="17"/>
+      <c r="AK33" s="17"/>
+      <c r="AL33" s="17"/>
+      <c r="AM33" s="17"/>
+      <c r="AN33" s="17"/>
+      <c r="AO33" s="17"/>
+      <c r="AP33" s="17"/>
+      <c r="AQ33" s="17"/>
+      <c r="AR33" s="17"/>
+      <c r="AS33" s="17"/>
+      <c r="AT33" s="17"/>
+      <c r="AU33" s="17"/>
+      <c r="AV33" s="17"/>
+      <c r="AW33" s="17"/>
+      <c r="AX33" s="17"/>
+      <c r="AY33" s="17"/>
+      <c r="AZ33" s="17"/>
+      <c r="BA33" s="17"/>
+      <c r="BB33" s="17"/>
+      <c r="BC33" s="17"/>
+      <c r="BD33" s="17"/>
+      <c r="BE33" s="17"/>
+      <c r="BF33" s="17"/>
+      <c r="BG33" s="17"/>
+      <c r="BH33" s="17"/>
+      <c r="BI33" s="17"/>
+      <c r="BJ33" s="17"/>
+      <c r="BK33" s="17"/>
+      <c r="BL33" s="17"/>
+      <c r="BM33" s="17"/>
+      <c r="BN33" s="17"/>
+      <c r="BO33" s="17"/>
+      <c r="BP33" s="17"/>
+      <c r="BQ33" s="17"/>
+      <c r="BR33" s="17"/>
+      <c r="BS33" s="17"/>
+      <c r="BT33" s="17"/>
+      <c r="BU33" s="17"/>
+      <c r="BV33" s="17"/>
+      <c r="BW33" s="17"/>
+      <c r="BX33" s="17"/>
+      <c r="BY33" s="17"/>
+      <c r="BZ33" s="17"/>
+      <c r="CA33" s="17"/>
+      <c r="CB33" s="17"/>
+      <c r="CC33" s="17"/>
+      <c r="CD33" s="17"/>
+      <c r="CE33" s="17"/>
+      <c r="CF33" s="17"/>
+      <c r="CG33" s="17"/>
+      <c r="CH33" s="17"/>
+      <c r="CI33" s="17"/>
+      <c r="CJ33" s="17"/>
+      <c r="CK33" s="17"/>
+      <c r="CL33" s="17"/>
+      <c r="CM33" s="17"/>
+      <c r="CN33" s="17"/>
+      <c r="CO33" s="17"/>
+      <c r="CP33" s="17"/>
+      <c r="CQ33" s="17"/>
+      <c r="CR33" s="17"/>
+      <c r="CS33" s="17"/>
+      <c r="CT33" s="17"/>
+      <c r="CU33" s="17"/>
+      <c r="CV33" s="17"/>
+      <c r="CW33" s="17"/>
+      <c r="CX33" s="17"/>
+      <c r="CY33" s="17"/>
+      <c r="CZ33" s="17"/>
+      <c r="DA33" s="17"/>
+      <c r="DB33" s="17"/>
+      <c r="DC33" s="17"/>
+      <c r="DD33" s="17"/>
+      <c r="DE33" s="17"/>
+      <c r="DF33" s="17"/>
+      <c r="DG33" s="17"/>
+      <c r="DH33" s="17"/>
+      <c r="DI33" s="17"/>
+      <c r="DJ33" s="17"/>
+      <c r="DK33" s="17"/>
+      <c r="DL33" s="17"/>
+      <c r="DM33" s="17"/>
+      <c r="DN33" s="17"/>
+      <c r="DO33" s="17"/>
+      <c r="DP33" s="17"/>
+      <c r="DQ33" s="17"/>
+      <c r="DR33" s="17"/>
+      <c r="DS33" s="17"/>
+      <c r="DT33" s="17"/>
+      <c r="DU33" s="17"/>
+      <c r="DV33" s="17"/>
+      <c r="DW33" s="17"/>
+      <c r="DX33" s="17"/>
+      <c r="DY33" s="17"/>
+      <c r="DZ33" s="17"/>
+      <c r="EA33" s="17"/>
+      <c r="EB33" s="17"/>
+      <c r="EC33" s="17"/>
+      <c r="ED33" s="17"/>
+      <c r="EE33" s="17"/>
+      <c r="EF33" s="17"/>
+      <c r="EG33" s="17"/>
+      <c r="EH33" s="17"/>
+      <c r="EI33" s="17"/>
+      <c r="EJ33" s="17"/>
+      <c r="EK33" s="17"/>
+      <c r="EL33" s="17"/>
+      <c r="EM33" s="17"/>
+      <c r="EN33" s="17"/>
+      <c r="EO33" s="17"/>
+      <c r="EP33" s="17"/>
+      <c r="EQ33" s="17"/>
+      <c r="ER33" s="17"/>
+      <c r="ES33" s="17"/>
+      <c r="ET33" s="17"/>
+      <c r="EU33" s="17"/>
+      <c r="EV33" s="17"/>
+      <c r="EW33" s="17"/>
+      <c r="EX33" s="17"/>
+      <c r="EY33" s="17"/>
+      <c r="EZ33" s="17"/>
+      <c r="FA33" s="17"/>
+      <c r="FB33" s="17"/>
+      <c r="FC33" s="17"/>
+      <c r="FD33" s="17"/>
+      <c r="FE33" s="17"/>
+      <c r="FF33" s="17"/>
+      <c r="FG33" s="17"/>
+      <c r="FH33" s="17"/>
+      <c r="FI33" s="17"/>
+      <c r="FJ33" s="17"/>
+      <c r="FK33" s="17"/>
+      <c r="FL33" s="17"/>
+      <c r="FM33" s="17"/>
+      <c r="FN33" s="17"/>
+      <c r="FO33" s="17"/>
+      <c r="FP33" s="17"/>
+      <c r="FQ33" s="17"/>
+      <c r="FR33" s="17"/>
+      <c r="FS33" s="17"/>
+      <c r="FT33" s="17"/>
+      <c r="FU33" s="17"/>
+      <c r="FV33" s="17"/>
+      <c r="FW33" s="17"/>
+      <c r="FX33" s="17"/>
+      <c r="FY33" s="17"/>
+      <c r="FZ33" s="17"/>
+      <c r="GA33" s="17"/>
+      <c r="GB33" s="17"/>
+      <c r="GC33" s="17"/>
+      <c r="GD33" s="17"/>
+      <c r="GE33" s="17"/>
+      <c r="GF33" s="17"/>
+      <c r="GG33" s="17"/>
+      <c r="GH33" s="17"/>
+      <c r="GI33" s="17"/>
+      <c r="GJ33" s="17"/>
+      <c r="GK33" s="17"/>
+      <c r="GL33" s="17"/>
+      <c r="GM33" s="17"/>
+      <c r="GN33" s="17"/>
+      <c r="GO33" s="17"/>
+      <c r="GP33" s="17"/>
+      <c r="GQ33" s="17"/>
+      <c r="GR33" s="17"/>
+      <c r="GS33" s="17"/>
+      <c r="GT33" s="17"/>
+      <c r="GU33" s="17"/>
+      <c r="GV33" s="17"/>
+      <c r="GW33" s="17"/>
+      <c r="GX33" s="17"/>
+      <c r="GY33" s="17"/>
+      <c r="GZ33" s="17"/>
+      <c r="HA33" s="17"/>
+      <c r="HB33" s="17"/>
+      <c r="HC33" s="17"/>
+      <c r="HD33" s="17"/>
+      <c r="HE33" s="17"/>
+      <c r="HF33" s="17"/>
+      <c r="HG33" s="17"/>
+      <c r="HH33" s="17"/>
+      <c r="HI33" s="17"/>
+      <c r="HJ33" s="17"/>
+      <c r="HK33" s="17"/>
+      <c r="HL33" s="17"/>
+      <c r="HM33" s="17"/>
+      <c r="HN33" s="17"/>
+      <c r="HO33" s="17"/>
+      <c r="HP33" s="17"/>
+      <c r="HQ33" s="17"/>
+      <c r="HR33" s="17"/>
+      <c r="HS33" s="17"/>
+      <c r="HT33" s="17"/>
+      <c r="HU33" s="17"/>
+      <c r="HV33" s="17"/>
+      <c r="HW33" s="17"/>
+      <c r="HX33" s="17"/>
+      <c r="HY33" s="17"/>
+      <c r="HZ33" s="17"/>
+      <c r="IA33" s="17"/>
+      <c r="IB33" s="17"/>
+      <c r="IC33" s="17"/>
+      <c r="ID33" s="17"/>
+      <c r="IE33" s="17"/>
+      <c r="IF33" s="17"/>
+      <c r="IG33" s="17"/>
+      <c r="IH33" s="17"/>
+      <c r="II33" s="17"/>
+      <c r="IJ33" s="17"/>
+      <c r="IK33" s="17"/>
+      <c r="IL33" s="17"/>
+      <c r="IM33" s="17"/>
+      <c r="IN33" s="17"/>
+      <c r="IO33" s="17"/>
+      <c r="IP33" s="17"/>
+      <c r="IQ33" s="17"/>
+      <c r="IR33" s="17"/>
+      <c r="IS33" s="17"/>
+      <c r="IT33" s="17"/>
+      <c r="IU33" s="17"/>
+      <c r="IV33" s="17"/>
+      <c r="IW33" s="17"/>
+      <c r="IX33" s="17"/>
+      <c r="IY33" s="17"/>
+      <c r="IZ33" s="17"/>
+      <c r="JA33" s="17"/>
+      <c r="JB33" s="17"/>
+      <c r="JC33" s="17"/>
+      <c r="JD33" s="17"/>
+      <c r="JE33" s="17"/>
+      <c r="JF33" s="17"/>
+      <c r="JG33" s="17"/>
+      <c r="JH33" s="17"/>
+      <c r="JI33" s="17"/>
+      <c r="JJ33" s="17"/>
+      <c r="JK33" s="17"/>
+      <c r="JL33" s="17"/>
+      <c r="JM33" s="17"/>
+      <c r="JN33" s="17"/>
+      <c r="JO33" s="17"/>
+      <c r="JP33" s="17"/>
+      <c r="JQ33" s="17"/>
+      <c r="JR33" s="17"/>
+      <c r="JS33" s="17"/>
+      <c r="JT33" s="17"/>
+      <c r="JU33" s="17"/>
+      <c r="JV33" s="17"/>
+      <c r="JW33" s="17"/>
+      <c r="JX33" s="17"/>
+      <c r="JY33" s="17"/>
+      <c r="JZ33" s="17"/>
+      <c r="KA33" s="17"/>
+      <c r="KB33" s="17"/>
+      <c r="KC33" s="17"/>
+      <c r="KD33" s="17"/>
+      <c r="KE33" s="17"/>
+      <c r="KF33" s="17"/>
+      <c r="KG33" s="17"/>
+      <c r="KH33" s="17"/>
+      <c r="KI33" s="17"/>
+      <c r="KJ33" s="17"/>
+      <c r="KK33" s="17"/>
+      <c r="KL33" s="17"/>
+      <c r="KM33" s="17"/>
+      <c r="KN33" s="17"/>
+      <c r="KO33" s="17"/>
+      <c r="KP33" s="17"/>
+      <c r="KQ33" s="17"/>
+      <c r="KR33" s="17"/>
+      <c r="KS33" s="17"/>
+      <c r="KT33" s="17"/>
+      <c r="KU33" s="17"/>
+      <c r="KV33" s="17"/>
+      <c r="KW33" s="17"/>
+      <c r="KX33" s="17"/>
+      <c r="KY33" s="17"/>
+      <c r="KZ33" s="17"/>
+      <c r="LA33" s="17"/>
+      <c r="LB33" s="17"/>
+      <c r="LC33" s="17"/>
+      <c r="LD33" s="17"/>
+      <c r="LE33" s="17"/>
+      <c r="LF33" s="17"/>
+      <c r="LG33" s="17"/>
+      <c r="LH33" s="17"/>
+      <c r="LI33" s="17"/>
+      <c r="LJ33" s="17"/>
+      <c r="LK33" s="17"/>
+      <c r="LL33" s="17"/>
+      <c r="LM33" s="17"/>
+      <c r="LN33" s="17"/>
+      <c r="LO33" s="17"/>
+      <c r="LP33" s="17"/>
+      <c r="LQ33" s="17"/>
+      <c r="LR33" s="17"/>
+      <c r="LS33" s="17"/>
+      <c r="LT33" s="17"/>
+      <c r="LU33" s="17"/>
+      <c r="LV33" s="17"/>
+      <c r="LW33" s="17"/>
+      <c r="LX33" s="17"/>
+      <c r="LY33" s="17"/>
+      <c r="LZ33" s="17"/>
+      <c r="MA33" s="17"/>
+      <c r="MB33" s="17"/>
+      <c r="MC33" s="17"/>
+      <c r="MD33" s="17"/>
+      <c r="ME33" s="17"/>
+      <c r="MF33" s="17"/>
+      <c r="MG33" s="17"/>
+      <c r="MH33" s="17"/>
+      <c r="MI33" s="17"/>
+      <c r="MJ33" s="17"/>
+      <c r="MK33" s="17"/>
+      <c r="ML33" s="17"/>
+      <c r="MM33" s="17"/>
+      <c r="MN33" s="17"/>
+      <c r="MO33" s="17"/>
+      <c r="MP33" s="17"/>
+      <c r="MQ33" s="17"/>
+      <c r="MR33" s="17"/>
+      <c r="MS33" s="17"/>
+      <c r="MT33" s="17"/>
+      <c r="MU33" s="17"/>
+      <c r="MV33" s="17"/>
+      <c r="MW33" s="17"/>
+      <c r="MX33" s="17"/>
+      <c r="MY33" s="17"/>
+      <c r="MZ33" s="17"/>
+      <c r="NA33" s="17"/>
+      <c r="NB33" s="17"/>
+      <c r="NC33" s="17"/>
+      <c r="ND33" s="17"/>
+      <c r="NE33" s="17"/>
+      <c r="NF33" s="17"/>
+      <c r="NG33" s="17"/>
+      <c r="NH33" s="17"/>
+      <c r="NI33" s="17"/>
+      <c r="NJ33" s="17"/>
+      <c r="NK33" s="17"/>
+      <c r="NL33" s="17"/>
+      <c r="NM33" s="17"/>
+      <c r="NN33" s="17"/>
+      <c r="NO33" s="17"/>
+      <c r="NP33" s="17"/>
+      <c r="NQ33" s="17"/>
+      <c r="NR33" s="17"/>
+      <c r="NS33" s="17"/>
+      <c r="NT33" s="17"/>
+      <c r="NU33" s="17"/>
+      <c r="NV33" s="17"/>
+      <c r="NW33" s="17"/>
+      <c r="NX33" s="17"/>
+      <c r="NY33" s="17"/>
+      <c r="NZ33" s="17"/>
+      <c r="OA33" s="17"/>
+      <c r="OB33" s="17"/>
+      <c r="OC33" s="17"/>
+      <c r="OD33" s="17"/>
+      <c r="OE33" s="17"/>
+      <c r="OF33" s="17"/>
+      <c r="OG33" s="17"/>
+      <c r="OH33" s="17"/>
+      <c r="OI33" s="17"/>
+      <c r="OJ33" s="17"/>
+      <c r="OK33" s="17"/>
+      <c r="OL33" s="17"/>
+      <c r="OM33" s="17"/>
+      <c r="ON33" s="17"/>
+      <c r="OO33" s="17"/>
+      <c r="OP33" s="17"/>
+      <c r="OQ33" s="17"/>
+      <c r="OR33" s="17"/>
+      <c r="OS33" s="17"/>
+      <c r="OT33" s="17"/>
+      <c r="OU33" s="17"/>
+      <c r="OV33" s="17"/>
+      <c r="OW33" s="17"/>
+      <c r="OX33" s="17"/>
+      <c r="OY33" s="17"/>
+      <c r="OZ33" s="17"/>
+      <c r="PA33" s="17"/>
+      <c r="PB33" s="17"/>
+      <c r="PC33" s="17"/>
+      <c r="PD33" s="17"/>
+      <c r="PE33" s="17"/>
+      <c r="PF33" s="17"/>
+      <c r="PG33" s="17"/>
+      <c r="PH33" s="17"/>
+      <c r="PI33" s="17"/>
+      <c r="PJ33" s="17"/>
+      <c r="PK33" s="17"/>
+      <c r="PL33" s="17"/>
+      <c r="PM33" s="17"/>
+      <c r="PN33" s="17"/>
+      <c r="PO33" s="17"/>
+      <c r="PP33" s="17"/>
+      <c r="PQ33" s="17"/>
+      <c r="PR33" s="17"/>
+      <c r="PS33" s="17"/>
+      <c r="PT33" s="17"/>
+      <c r="PU33" s="17"/>
+      <c r="PV33" s="17"/>
+      <c r="PW33" s="17"/>
+      <c r="PX33" s="17"/>
+      <c r="PY33" s="17"/>
+      <c r="PZ33" s="17"/>
+      <c r="QA33" s="17"/>
+      <c r="QB33" s="17"/>
+      <c r="QC33" s="17"/>
+      <c r="QD33" s="17"/>
+      <c r="QE33" s="17"/>
+      <c r="QF33" s="17"/>
+      <c r="QG33" s="17"/>
+      <c r="QH33" s="17"/>
+      <c r="QI33" s="17"/>
+      <c r="QJ33" s="17"/>
+      <c r="QK33" s="17"/>
+      <c r="QL33" s="17"/>
+      <c r="QM33" s="17"/>
+      <c r="QN33" s="17"/>
+      <c r="QO33" s="17"/>
+      <c r="QP33" s="17"/>
+      <c r="QQ33" s="17"/>
+      <c r="QR33" s="17"/>
+      <c r="QS33" s="17"/>
+      <c r="QT33" s="17"/>
+      <c r="QU33" s="17"/>
+      <c r="QV33" s="17"/>
+      <c r="QW33" s="17"/>
+      <c r="QX33" s="17"/>
+      <c r="QY33" s="17"/>
+      <c r="QZ33" s="17"/>
+      <c r="RA33" s="17"/>
+      <c r="RB33" s="17"/>
+      <c r="RC33" s="17"/>
+      <c r="RD33" s="17"/>
+      <c r="RE33" s="17"/>
+      <c r="RF33" s="17"/>
+      <c r="RG33" s="17"/>
+      <c r="RH33" s="17"/>
+      <c r="RI33" s="17"/>
+      <c r="RJ33" s="17"/>
+      <c r="RK33" s="17"/>
+      <c r="RL33" s="17"/>
+      <c r="RM33" s="17"/>
+      <c r="RN33" s="17"/>
+      <c r="RO33" s="17"/>
+      <c r="RP33" s="17"/>
+      <c r="RQ33" s="17"/>
+      <c r="RR33" s="17"/>
+      <c r="RS33" s="17"/>
+      <c r="RT33" s="17"/>
+      <c r="RU33" s="17"/>
+      <c r="RV33" s="17"/>
+      <c r="RW33" s="17"/>
+      <c r="RX33" s="17"/>
+      <c r="RY33" s="17"/>
+      <c r="RZ33" s="17"/>
+      <c r="SA33" s="17"/>
+      <c r="SB33" s="17"/>
+      <c r="SC33" s="17"/>
+      <c r="SD33" s="17"/>
+      <c r="SE33" s="17"/>
+      <c r="SF33" s="17"/>
+      <c r="SG33" s="17"/>
+      <c r="SH33" s="17"/>
+      <c r="SI33" s="17"/>
+      <c r="SJ33" s="17"/>
+      <c r="SK33" s="17"/>
+      <c r="SL33" s="17"/>
+      <c r="SM33" s="17"/>
+      <c r="SN33" s="17"/>
+      <c r="SO33" s="17"/>
+      <c r="SP33" s="17"/>
+      <c r="SQ33" s="17"/>
+      <c r="SR33" s="17"/>
+      <c r="SS33" s="17"/>
+      <c r="ST33" s="17"/>
+      <c r="SU33" s="17"/>
+      <c r="SV33" s="17"/>
+      <c r="SW33" s="17"/>
+      <c r="SX33" s="17"/>
+      <c r="SY33" s="17"/>
+      <c r="SZ33" s="17"/>
+      <c r="TA33" s="17"/>
+      <c r="TB33" s="17"/>
+      <c r="TC33" s="17"/>
+      <c r="TD33" s="17"/>
+      <c r="TE33" s="17"/>
+      <c r="TF33" s="17"/>
+      <c r="TG33" s="17"/>
+      <c r="TH33" s="17"/>
+      <c r="TI33" s="17"/>
+      <c r="TJ33" s="17"/>
+      <c r="TK33" s="17"/>
+      <c r="TL33" s="17"/>
+      <c r="TM33" s="17"/>
+      <c r="TN33" s="17"/>
+      <c r="TO33" s="17"/>
+      <c r="TP33" s="17"/>
+      <c r="TQ33" s="17"/>
+      <c r="TR33" s="17"/>
+      <c r="TS33" s="17"/>
+      <c r="TT33" s="17"/>
+      <c r="TU33" s="17"/>
+      <c r="TV33" s="17"/>
+      <c r="TW33" s="17"/>
+      <c r="TX33" s="17"/>
+      <c r="TY33" s="17"/>
+      <c r="TZ33" s="17"/>
+      <c r="UA33" s="17"/>
+      <c r="UB33" s="17"/>
+      <c r="UC33" s="17"/>
+      <c r="UD33" s="17"/>
+      <c r="UE33" s="17"/>
+      <c r="UF33" s="17"/>
+      <c r="UG33" s="17"/>
+      <c r="UH33" s="17"/>
+      <c r="UI33" s="17"/>
+      <c r="UJ33" s="17"/>
+      <c r="UK33" s="17"/>
+      <c r="UL33" s="17"/>
+      <c r="UM33" s="17"/>
+      <c r="UN33" s="17"/>
+      <c r="UO33" s="17"/>
+      <c r="UP33" s="17"/>
+      <c r="UQ33" s="17"/>
+      <c r="UR33" s="17"/>
+      <c r="US33" s="17"/>
+      <c r="UT33" s="17"/>
+      <c r="UU33" s="17"/>
+      <c r="UV33" s="17"/>
+      <c r="UW33" s="17"/>
+      <c r="UX33" s="17"/>
+      <c r="UY33" s="17"/>
+      <c r="UZ33" s="17"/>
+      <c r="VA33" s="17"/>
+      <c r="VB33" s="17"/>
+      <c r="VC33" s="17"/>
+      <c r="VD33" s="17"/>
+      <c r="VE33" s="17"/>
+      <c r="VF33" s="17"/>
+      <c r="VG33" s="17"/>
+      <c r="VH33" s="17"/>
+      <c r="VI33" s="17"/>
+      <c r="VJ33" s="17"/>
+      <c r="VK33" s="17"/>
+      <c r="VL33" s="17"/>
+      <c r="VM33" s="17"/>
+      <c r="VN33" s="17"/>
+      <c r="VO33" s="17"/>
+      <c r="VP33" s="17"/>
+      <c r="VQ33" s="17"/>
+      <c r="VR33" s="17"/>
+      <c r="VS33" s="17"/>
+      <c r="VT33" s="17"/>
+      <c r="VU33" s="17"/>
+      <c r="VV33" s="17"/>
+      <c r="VW33" s="17"/>
+      <c r="VX33" s="17"/>
+      <c r="VY33" s="17"/>
+      <c r="VZ33" s="17"/>
+      <c r="WA33" s="17"/>
+      <c r="WB33" s="17"/>
+      <c r="WC33" s="17"/>
+      <c r="WD33" s="17"/>
+      <c r="WE33" s="17"/>
+      <c r="WF33" s="17"/>
+      <c r="WG33" s="17"/>
+      <c r="WH33" s="17"/>
+      <c r="WI33" s="17"/>
+      <c r="WJ33" s="17"/>
+      <c r="WK33" s="17"/>
+      <c r="WL33" s="17"/>
+      <c r="WM33" s="17"/>
+      <c r="WN33" s="17"/>
+      <c r="WO33" s="17"/>
+      <c r="WP33" s="17"/>
+      <c r="WQ33" s="17"/>
+      <c r="WR33" s="17"/>
+      <c r="WS33" s="17"/>
+      <c r="WT33" s="17"/>
+      <c r="WU33" s="17"/>
+      <c r="WV33" s="17"/>
+      <c r="WW33" s="17"/>
+      <c r="WX33" s="17"/>
+      <c r="WY33" s="17"/>
+      <c r="WZ33" s="17"/>
+      <c r="XA33" s="17"/>
+      <c r="XB33" s="17"/>
+      <c r="XC33" s="17"/>
+      <c r="XD33" s="17"/>
+      <c r="XE33" s="17"/>
+      <c r="XF33" s="17"/>
+      <c r="XG33" s="17"/>
+      <c r="XH33" s="17"/>
+      <c r="XI33" s="17"/>
+      <c r="XJ33" s="17"/>
+      <c r="XK33" s="17"/>
+      <c r="XL33" s="17"/>
+      <c r="XM33" s="17"/>
+      <c r="XN33" s="17"/>
+      <c r="XO33" s="17"/>
+      <c r="XP33" s="17"/>
+      <c r="XQ33" s="17"/>
+      <c r="XR33" s="17"/>
+      <c r="XS33" s="17"/>
+      <c r="XT33" s="17"/>
+      <c r="XU33" s="17"/>
+      <c r="XV33" s="17"/>
+      <c r="XW33" s="17"/>
+      <c r="XX33" s="17"/>
+      <c r="XY33" s="17"/>
+      <c r="XZ33" s="17"/>
+      <c r="YA33" s="17"/>
+      <c r="YB33" s="17"/>
+      <c r="YC33" s="17"/>
+      <c r="YD33" s="17"/>
+      <c r="YE33" s="17"/>
+      <c r="YF33" s="17"/>
+      <c r="YG33" s="17"/>
+      <c r="YH33" s="17"/>
+      <c r="YI33" s="17"/>
+      <c r="YJ33" s="17"/>
+      <c r="YK33" s="17"/>
+      <c r="YL33" s="17"/>
+      <c r="YM33" s="17"/>
+      <c r="YN33" s="17"/>
+      <c r="YO33" s="17"/>
+      <c r="YP33" s="17"/>
+      <c r="YQ33" s="17"/>
+      <c r="YR33" s="17"/>
+      <c r="YS33" s="17"/>
+      <c r="YT33" s="17"/>
+      <c r="YU33" s="17"/>
+      <c r="YV33" s="17"/>
+      <c r="YW33" s="17"/>
+      <c r="YX33" s="17"/>
+      <c r="YY33" s="17"/>
+      <c r="YZ33" s="17"/>
+      <c r="ZA33" s="17"/>
+      <c r="ZB33" s="17"/>
+      <c r="ZC33" s="17"/>
+      <c r="ZD33" s="17"/>
+      <c r="ZE33" s="17"/>
+      <c r="ZF33" s="17"/>
+      <c r="ZG33" s="17"/>
+      <c r="ZH33" s="17"/>
+      <c r="ZI33" s="17"/>
+      <c r="ZJ33" s="17"/>
+      <c r="ZK33" s="17"/>
+      <c r="ZL33" s="17"/>
+      <c r="ZM33" s="17"/>
+      <c r="ZN33" s="17"/>
+      <c r="ZO33" s="17"/>
+      <c r="ZP33" s="17"/>
+      <c r="ZQ33" s="17"/>
+      <c r="ZR33" s="17"/>
+      <c r="ZS33" s="17"/>
+      <c r="ZT33" s="17"/>
+      <c r="ZU33" s="17"/>
+      <c r="ZV33" s="17"/>
+      <c r="ZW33" s="17"/>
+      <c r="ZX33" s="17"/>
+      <c r="ZY33" s="17"/>
+      <c r="ZZ33" s="17"/>
+      <c r="AAA33" s="17"/>
+      <c r="AAB33" s="17"/>
+      <c r="AAC33" s="17"/>
+      <c r="AAD33" s="17"/>
+      <c r="AAE33" s="17"/>
+      <c r="AAF33" s="17"/>
+      <c r="AAG33" s="17"/>
+      <c r="AAH33" s="17"/>
+      <c r="AAI33" s="17"/>
+      <c r="AAJ33" s="17"/>
+      <c r="AAK33" s="17"/>
+      <c r="AAL33" s="17"/>
+      <c r="AAM33" s="17"/>
+      <c r="AAN33" s="17"/>
+      <c r="AAO33" s="17"/>
+      <c r="AAP33" s="17"/>
+      <c r="AAQ33" s="17"/>
+      <c r="AAR33" s="17"/>
+      <c r="AAS33" s="17"/>
+      <c r="AAT33" s="17"/>
+      <c r="AAU33" s="17"/>
+      <c r="AAV33" s="17"/>
+      <c r="AAW33" s="17"/>
+      <c r="AAX33" s="17"/>
+      <c r="AAY33" s="17"/>
+      <c r="AAZ33" s="17"/>
+      <c r="ABA33" s="17"/>
+      <c r="ABB33" s="17"/>
+      <c r="ABC33" s="17"/>
+      <c r="ABD33" s="17"/>
+      <c r="ABE33" s="17"/>
+      <c r="ABF33" s="17"/>
+      <c r="ABG33" s="17"/>
+      <c r="ABH33" s="17"/>
+      <c r="ABI33" s="17"/>
+      <c r="ABJ33" s="17"/>
+      <c r="ABK33" s="17"/>
+      <c r="ABL33" s="17"/>
+      <c r="ABM33" s="17"/>
+      <c r="ABN33" s="17"/>
+      <c r="ABO33" s="17"/>
+      <c r="ABP33" s="17"/>
+      <c r="ABQ33" s="17"/>
+      <c r="ABR33" s="17"/>
+      <c r="ABS33" s="17"/>
+      <c r="ABT33" s="17"/>
+      <c r="ABU33" s="17"/>
+      <c r="ABV33" s="17"/>
+      <c r="ABW33" s="17"/>
+      <c r="ABX33" s="17"/>
+      <c r="ABY33" s="17"/>
+      <c r="ABZ33" s="17"/>
+      <c r="ACA33" s="17"/>
+      <c r="ACB33" s="17"/>
+      <c r="ACC33" s="17"/>
+      <c r="ACD33" s="17"/>
+      <c r="ACE33" s="17"/>
+      <c r="ACF33" s="17"/>
+      <c r="ACG33" s="17"/>
+      <c r="ACH33" s="17"/>
+      <c r="ACI33" s="17"/>
+      <c r="ACJ33" s="17"/>
+      <c r="ACK33" s="17"/>
+      <c r="ACL33" s="17"/>
+      <c r="ACM33" s="17"/>
+      <c r="ACN33" s="17"/>
+      <c r="ACO33" s="17"/>
+      <c r="ACP33" s="17"/>
+      <c r="ACQ33" s="17"/>
+      <c r="ACR33" s="17"/>
+      <c r="ACS33" s="17"/>
+      <c r="ACT33" s="17"/>
+      <c r="ACU33" s="17"/>
+      <c r="ACV33" s="17"/>
+      <c r="ACW33" s="17"/>
+      <c r="ACX33" s="17"/>
+      <c r="ACY33" s="17"/>
+      <c r="ACZ33" s="17"/>
+      <c r="ADA33" s="17"/>
+      <c r="ADB33" s="17"/>
+      <c r="ADC33" s="17"/>
+      <c r="ADD33" s="17"/>
+      <c r="ADE33" s="17"/>
+      <c r="ADF33" s="17"/>
+      <c r="ADG33" s="17"/>
+      <c r="ADH33" s="17"/>
+      <c r="ADI33" s="17"/>
+      <c r="ADJ33" s="17"/>
+      <c r="ADK33" s="17"/>
+      <c r="ADL33" s="17"/>
+      <c r="ADM33" s="17"/>
+      <c r="ADN33" s="17"/>
+      <c r="ADO33" s="17"/>
+      <c r="ADP33" s="17"/>
+      <c r="ADQ33" s="17"/>
+      <c r="ADR33" s="17"/>
+      <c r="ADS33" s="17"/>
+      <c r="ADT33" s="17"/>
+      <c r="ADU33" s="17"/>
+      <c r="ADV33" s="17"/>
+      <c r="ADW33" s="17"/>
+      <c r="ADX33" s="17"/>
+      <c r="ADY33" s="17"/>
+      <c r="ADZ33" s="17"/>
+      <c r="AEA33" s="17"/>
+      <c r="AEB33" s="17"/>
+      <c r="AEC33" s="17"/>
+      <c r="AED33" s="17"/>
+      <c r="AEE33" s="17"/>
+      <c r="AEF33" s="17"/>
+      <c r="AEG33" s="17"/>
+      <c r="AEH33" s="17"/>
+      <c r="AEI33" s="17"/>
+      <c r="AEJ33" s="17"/>
+      <c r="AEK33" s="17"/>
+      <c r="AEL33" s="17"/>
+      <c r="AEM33" s="17"/>
+      <c r="AEN33" s="17"/>
+      <c r="AEO33" s="17"/>
+      <c r="AEP33" s="17"/>
+      <c r="AEQ33" s="17"/>
+      <c r="AER33" s="17"/>
+      <c r="AES33" s="17"/>
+      <c r="AET33" s="17"/>
+      <c r="AEU33" s="17"/>
+      <c r="AEV33" s="17"/>
+      <c r="AEW33" s="17"/>
+      <c r="AEX33" s="17"/>
+      <c r="AEY33" s="17"/>
+      <c r="AEZ33" s="17"/>
+      <c r="AFA33" s="17"/>
+      <c r="AFB33" s="17"/>
+      <c r="AFC33" s="17"/>
+      <c r="AFD33" s="17"/>
+      <c r="AFE33" s="17"/>
+      <c r="AFF33" s="17"/>
+      <c r="AFG33" s="17"/>
+      <c r="AFH33" s="17"/>
+      <c r="AFI33" s="17"/>
+      <c r="AFJ33" s="17"/>
+      <c r="AFK33" s="17"/>
+      <c r="AFL33" s="17"/>
+      <c r="AFM33" s="17"/>
+      <c r="AFN33" s="17"/>
+      <c r="AFO33" s="17"/>
+      <c r="AFP33" s="17"/>
+      <c r="AFQ33" s="17"/>
+      <c r="AFR33" s="17"/>
+      <c r="AFS33" s="17"/>
+      <c r="AFT33" s="17"/>
+      <c r="AFU33" s="17"/>
+      <c r="AFV33" s="17"/>
+      <c r="AFW33" s="17"/>
+      <c r="AFX33" s="17"/>
+      <c r="AFY33" s="17"/>
+      <c r="AFZ33" s="17"/>
+      <c r="AGA33" s="17"/>
+      <c r="AGB33" s="17"/>
+      <c r="AGC33" s="17"/>
+      <c r="AGD33" s="17"/>
+      <c r="AGE33" s="17"/>
+      <c r="AGF33" s="17"/>
+      <c r="AGG33" s="17"/>
+      <c r="AGH33" s="17"/>
+      <c r="AGI33" s="17"/>
+      <c r="AGJ33" s="17"/>
+      <c r="AGK33" s="17"/>
+      <c r="AGL33" s="17"/>
+      <c r="AGM33" s="17"/>
+      <c r="AGN33" s="17"/>
+      <c r="AGO33" s="17"/>
+      <c r="AGP33" s="17"/>
+      <c r="AGQ33" s="17"/>
+      <c r="AGR33" s="17"/>
+      <c r="AGS33" s="17"/>
+      <c r="AGT33" s="17"/>
+      <c r="AGU33" s="17"/>
+      <c r="AGV33" s="17"/>
+      <c r="AGW33" s="17"/>
+      <c r="AGX33" s="17"/>
+      <c r="AGY33" s="17"/>
+      <c r="AGZ33" s="17"/>
+      <c r="AHA33" s="17"/>
+      <c r="AHB33" s="17"/>
+      <c r="AHC33" s="17"/>
+      <c r="AHD33" s="17"/>
+      <c r="AHE33" s="17"/>
+      <c r="AHF33" s="17"/>
+      <c r="AHG33" s="17"/>
+      <c r="AHH33" s="17"/>
+      <c r="AHI33" s="17"/>
+      <c r="AHJ33" s="17"/>
+      <c r="AHK33" s="17"/>
+      <c r="AHL33" s="17"/>
+      <c r="AHM33" s="17"/>
+      <c r="AHN33" s="17"/>
+      <c r="AHO33" s="17"/>
+      <c r="AHP33" s="17"/>
+      <c r="AHQ33" s="17"/>
+      <c r="AHR33" s="17"/>
+      <c r="AHS33" s="17"/>
+      <c r="AHT33" s="17"/>
+      <c r="AHU33" s="17"/>
+      <c r="AHV33" s="17"/>
+      <c r="AHW33" s="17"/>
+      <c r="AHX33" s="17"/>
+      <c r="AHY33" s="17"/>
+      <c r="AHZ33" s="17"/>
+      <c r="AIA33" s="17"/>
+      <c r="AIB33" s="17"/>
+      <c r="AIC33" s="17"/>
+      <c r="AID33" s="17"/>
+      <c r="AIE33" s="17"/>
+      <c r="AIF33" s="17"/>
+      <c r="AIG33" s="17"/>
+      <c r="AIH33" s="17"/>
+      <c r="AII33" s="17"/>
+      <c r="AIJ33" s="17"/>
+      <c r="AIK33" s="17"/>
+      <c r="AIL33" s="17"/>
+      <c r="AIM33" s="17"/>
+      <c r="AIN33" s="17"/>
+      <c r="AIO33" s="17"/>
+      <c r="AIP33" s="17"/>
+      <c r="AIQ33" s="17"/>
+      <c r="AIR33" s="17"/>
+      <c r="AIS33" s="17"/>
+      <c r="AIT33" s="17"/>
+      <c r="AIU33" s="17"/>
+      <c r="AIV33" s="17"/>
+      <c r="AIW33" s="17"/>
+      <c r="AIX33" s="17"/>
+      <c r="AIY33" s="17"/>
+      <c r="AIZ33" s="17"/>
+      <c r="AJA33" s="17"/>
+      <c r="AJB33" s="17"/>
+      <c r="AJC33" s="17"/>
+      <c r="AJD33" s="17"/>
+      <c r="AJE33" s="17"/>
+      <c r="AJF33" s="17"/>
+      <c r="AJG33" s="17"/>
+      <c r="AJH33" s="17"/>
+      <c r="AJI33" s="17"/>
+      <c r="AJJ33" s="17"/>
+      <c r="AJK33" s="17"/>
+      <c r="AJL33" s="17"/>
+      <c r="AJM33" s="17"/>
+      <c r="AJN33" s="17"/>
+      <c r="AJO33" s="17"/>
+      <c r="AJP33" s="17"/>
+      <c r="AJQ33" s="17"/>
+      <c r="AJR33" s="17"/>
+      <c r="AJS33" s="17"/>
+      <c r="AJT33" s="17"/>
+      <c r="AJU33" s="17"/>
+      <c r="AJV33" s="17"/>
+      <c r="AJW33" s="17"/>
+      <c r="AJX33" s="17"/>
+      <c r="AJY33" s="17"/>
+      <c r="AJZ33" s="17"/>
+      <c r="AKA33" s="17"/>
+      <c r="AKB33" s="17"/>
+      <c r="AKC33" s="17"/>
+      <c r="AKD33" s="17"/>
+      <c r="AKE33" s="17"/>
+      <c r="AKF33" s="17"/>
+      <c r="AKG33" s="17"/>
+      <c r="AKH33" s="17"/>
+      <c r="AKI33" s="17"/>
+      <c r="AKJ33" s="17"/>
+      <c r="AKK33" s="17"/>
+      <c r="AKL33" s="17"/>
+      <c r="AKM33" s="17"/>
+      <c r="AKN33" s="17"/>
+      <c r="AKO33" s="17"/>
+      <c r="AKP33" s="17"/>
+      <c r="AKQ33" s="17"/>
+      <c r="AKR33" s="17"/>
+      <c r="AKS33" s="17"/>
+      <c r="AKT33" s="17"/>
+      <c r="AKU33" s="17"/>
+      <c r="AKV33" s="17"/>
+      <c r="AKW33" s="17"/>
+      <c r="AKX33" s="17"/>
+      <c r="AKY33" s="17"/>
+      <c r="AKZ33" s="17"/>
+      <c r="ALA33" s="17"/>
+      <c r="ALB33" s="17"/>
+      <c r="ALC33" s="17"/>
+      <c r="ALD33" s="17"/>
+      <c r="ALE33" s="17"/>
+      <c r="ALF33" s="17"/>
+      <c r="ALG33" s="17"/>
+      <c r="ALH33" s="17"/>
+      <c r="ALI33" s="17"/>
+      <c r="ALJ33" s="17"/>
+      <c r="ALK33" s="17"/>
+      <c r="ALL33" s="17"/>
+      <c r="ALM33" s="17"/>
+      <c r="ALN33" s="17"/>
+      <c r="ALO33" s="17"/>
+      <c r="ALP33" s="17"/>
+      <c r="ALQ33" s="17"/>
+      <c r="ALR33" s="17"/>
+      <c r="ALS33" s="17"/>
+      <c r="ALT33" s="17"/>
+      <c r="ALU33" s="17"/>
+      <c r="ALV33" s="17"/>
+      <c r="ALW33" s="17"/>
+      <c r="ALX33" s="17"/>
+      <c r="ALY33" s="17"/>
+      <c r="ALZ33" s="17"/>
+      <c r="AMA33" s="17"/>
+      <c r="AMB33" s="17"/>
+      <c r="AMC33" s="17"/>
+      <c r="AMD33" s="17"/>
+      <c r="AME33" s="17"/>
+      <c r="AMF33" s="17"/>
+      <c r="AMG33" s="17"/>
+      <c r="AMH33" s="17"/>
+      <c r="AMI33" s="17"/>
+      <c r="AMJ33" s="17"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="2:1024">
       <c r="B35" s="55" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C35" s="56" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D35" s="56"/>
       <c r="E35" s="56"/>
       <c r="F35" s="57"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="2:1024">
       <c r="B36" s="55"/>
       <c r="C36" s="45" t="s">
         <v>18</v>
@@ -32775,60 +33727,71 @@
       </c>
       <c r="F36" s="57"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="2:1024">
       <c r="B37" s="42" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C37" s="46" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D37" s="46"/>
       <c r="E37" s="46"/>
       <c r="F37" s="42"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="2:1024">
       <c r="B38" s="42" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C38" s="46" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D38" s="46"/>
       <c r="E38" s="46"/>
       <c r="F38" s="42"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="2:1024">
       <c r="B39" s="42" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C39" s="46" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D39" s="46"/>
       <c r="E39" s="46"/>
       <c r="F39" s="42"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="2:1024">
       <c r="B40" s="42" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C40" s="46" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D40" s="46"/>
       <c r="E40" s="46"/>
       <c r="F40" s="42"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="2:1024">
       <c r="B41" s="42" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="C41" s="46" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D41" s="46"/>
       <c r="E41" s="46"/>
       <c r="F41" s="42"/>
+    </row>
+    <row r="42" spans="2:1024">
+      <c r="B42" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -32868,15 +33831,15 @@
     <row r="2" spans="2:1024" customFormat="1" ht="14.45" customHeight="1">
       <c r="B2" s="60"/>
       <c r="C2" s="61" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D2" s="62" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E2" s="63"/>
       <c r="F2" s="64"/>
       <c r="G2" s="65" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
@@ -33900,13 +34863,13 @@
       <c r="B3" s="60"/>
       <c r="C3" s="61"/>
       <c r="D3" s="25" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G3" s="65"/>
       <c r="H3" s="17"/>
@@ -35959,10 +36922,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
@@ -36990,10 +37953,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
@@ -38021,12 +38984,12 @@
         <v>3</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D7" s="30"/>
       <c r="E7" s="30"/>
       <c r="F7" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="G7" s="29"/>
       <c r="H7" s="17"/>
@@ -40079,10 +41042,10 @@
         <v>4</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E9" s="30"/>
       <c r="F9" s="30"/>
@@ -40093,10 +41056,10 @@
         <v>5</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="30"/>
@@ -40107,10 +41070,10 @@
         <v>6</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E11" s="30"/>
       <c r="F11" s="30"/>
@@ -40121,12 +41084,12 @@
         <v>7</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
       <c r="F12" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="G12" s="29"/>
     </row>
@@ -40145,12 +41108,12 @@
         <v>8</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
       <c r="F14" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="G14" s="29"/>
     </row>
@@ -40431,11 +41394,6 @@
     <row r="208" s="31" customFormat="1"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C65:F65"/>
-    <mergeCell ref="C75:F75"/>
-    <mergeCell ref="C98:F98"/>
-    <mergeCell ref="C110:F110"/>
-    <mergeCell ref="C126:F126"/>
     <mergeCell ref="C54:F54"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -40447,6 +41405,11 @@
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C33:F33"/>
     <mergeCell ref="C46:F46"/>
+    <mergeCell ref="C65:F65"/>
+    <mergeCell ref="C75:F75"/>
+    <mergeCell ref="C98:F98"/>
+    <mergeCell ref="C110:F110"/>
+    <mergeCell ref="C126:F126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -40456,10 +41419,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AMJ213"/>
+  <dimension ref="A2:AMJ211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="C1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -40475,28 +41438,28 @@
     <row r="2" spans="1:7" ht="14.45" customHeight="1">
       <c r="B2" s="60"/>
       <c r="C2" s="61" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D2" s="62" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E2" s="63"/>
       <c r="F2" s="64"/>
       <c r="G2" s="65" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="60"/>
       <c r="C3" s="61"/>
       <c r="D3" s="25" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G3" s="65"/>
     </row>
@@ -40515,10 +41478,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
@@ -40529,10 +41492,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
@@ -40543,10 +41506,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
@@ -40557,10 +41520,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
@@ -40582,10 +41545,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="30"/>
@@ -40596,10 +41559,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E11" s="30"/>
       <c r="F11" s="30"/>
@@ -40611,10 +41574,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
@@ -40626,10 +41589,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E13" s="30"/>
       <c r="F13" s="30"/>
@@ -40641,126 +41604,98 @@
         <v>5</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
       <c r="G14" s="29"/>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15"/>
-      <c r="B15" s="28">
-        <v>6</v>
+    <row r="15" spans="1:7" s="31" customFormat="1">
+      <c r="B15" s="66" t="s">
+        <v>14</v>
       </c>
-      <c r="C15" s="29" t="s">
-        <v>122</v>
+      <c r="C15" s="66"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+    </row>
+    <row r="16" spans="1:7" s="31" customFormat="1">
+      <c r="B16" s="28">
+        <v>1</v>
       </c>
-      <c r="D15" s="30" t="s">
-        <v>93</v>
+      <c r="C16" s="35" t="s">
+        <v>68</v>
       </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="29"/>
-    </row>
-    <row r="16" spans="1:7" ht="38.25">
-      <c r="A16"/>
-      <c r="B16" s="28">
-        <v>7</v>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30" t="s">
+        <v>102</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="29"/>
+      <c r="G16" s="36"/>
     </row>
     <row r="17" spans="2:7" s="31" customFormat="1">
-      <c r="B17" s="66" t="s">
-        <v>14</v>
+      <c r="B17" s="28">
+        <v>2</v>
       </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
+      <c r="C17" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="G17" s="29"/>
     </row>
     <row r="18" spans="2:7" s="31" customFormat="1">
       <c r="B18" s="28">
-        <v>1</v>
+        <v>3</v>
       </c>
-      <c r="C18" s="35" t="s">
-        <v>64</v>
+      <c r="C18" s="37" t="s">
+        <v>70</v>
       </c>
       <c r="D18" s="30"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
-      <c r="G18" s="36"/>
+      <c r="G18" s="29"/>
     </row>
     <row r="19" spans="2:7" s="31" customFormat="1">
       <c r="B19" s="28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D19" s="30"/>
       <c r="E19" s="30"/>
       <c r="F19" s="30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="G19" s="29"/>
     </row>
-    <row r="20" spans="2:7" s="31" customFormat="1">
-      <c r="B20" s="28">
-        <v>3</v>
-      </c>
-      <c r="C20" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="G20" s="29"/>
+    <row r="20" spans="2:7" s="31" customFormat="1"/>
+    <row r="21" spans="2:7" s="31" customFormat="1"/>
+    <row r="22" spans="2:7" s="31" customFormat="1"/>
+    <row r="23" spans="2:7" s="31" customFormat="1">
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
     </row>
-    <row r="21" spans="2:7" s="31" customFormat="1">
-      <c r="B21" s="28">
-        <v>4</v>
-      </c>
-      <c r="C21" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="G21" s="29"/>
-    </row>
-    <row r="22" spans="2:7" s="31" customFormat="1"/>
-    <row r="23" spans="2:7" s="31" customFormat="1"/>
     <row r="24" spans="2:7" s="31" customFormat="1"/>
     <row r="25" spans="2:7" s="31" customFormat="1">
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
     </row>
     <row r="26" spans="2:7" s="31" customFormat="1"/>
-    <row r="27" spans="2:7" s="31" customFormat="1">
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-    </row>
+    <row r="27" spans="2:7" s="31" customFormat="1"/>
     <row r="28" spans="2:7" s="31" customFormat="1"/>
     <row r="29" spans="2:7" s="31" customFormat="1"/>
     <row r="30" spans="2:7" s="31" customFormat="1"/>
@@ -40769,76 +41704,76 @@
     <row r="33" spans="3:6" s="31" customFormat="1"/>
     <row r="34" spans="3:6" s="31" customFormat="1"/>
     <row r="35" spans="3:6" s="31" customFormat="1"/>
-    <row r="36" spans="3:6" s="31" customFormat="1"/>
+    <row r="36" spans="3:6" s="31" customFormat="1">
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="59"/>
+    </row>
     <row r="37" spans="3:6" s="31" customFormat="1"/>
     <row r="38" spans="3:6" s="31" customFormat="1">
-      <c r="C38" s="59"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="59"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
     </row>
     <row r="39" spans="3:6" s="31" customFormat="1"/>
-    <row r="40" spans="3:6" s="31" customFormat="1">
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-    </row>
+    <row r="40" spans="3:6" s="31" customFormat="1"/>
     <row r="41" spans="3:6" s="31" customFormat="1"/>
     <row r="42" spans="3:6" s="31" customFormat="1"/>
     <row r="43" spans="3:6" s="31" customFormat="1"/>
-    <row r="44" spans="3:6" s="31" customFormat="1"/>
+    <row r="44" spans="3:6" s="31" customFormat="1">
+      <c r="C44" s="59"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="59"/>
+      <c r="F44" s="59"/>
+    </row>
     <row r="45" spans="3:6" s="31" customFormat="1"/>
     <row r="46" spans="3:6" s="31" customFormat="1">
-      <c r="C46" s="59"/>
-      <c r="D46" s="59"/>
-      <c r="E46" s="59"/>
-      <c r="F46" s="59"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="34"/>
     </row>
     <row r="47" spans="3:6" s="31" customFormat="1"/>
-    <row r="48" spans="3:6" s="31" customFormat="1">
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
-    </row>
+    <row r="48" spans="3:6" s="31" customFormat="1"/>
     <row r="49" spans="3:6" s="31" customFormat="1"/>
     <row r="50" spans="3:6" s="31" customFormat="1"/>
     <row r="51" spans="3:6" s="31" customFormat="1"/>
     <row r="52" spans="3:6" s="31" customFormat="1"/>
     <row r="53" spans="3:6" s="31" customFormat="1"/>
     <row r="54" spans="3:6" s="31" customFormat="1"/>
-    <row r="55" spans="3:6" s="31" customFormat="1"/>
+    <row r="55" spans="3:6" s="31" customFormat="1">
+      <c r="C55" s="59"/>
+      <c r="D55" s="59"/>
+      <c r="E55" s="59"/>
+      <c r="F55" s="59"/>
+    </row>
     <row r="56" spans="3:6" s="31" customFormat="1"/>
     <row r="57" spans="3:6" s="31" customFormat="1">
-      <c r="C57" s="59"/>
-      <c r="D57" s="59"/>
-      <c r="E57" s="59"/>
-      <c r="F57" s="59"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="34"/>
     </row>
     <row r="58" spans="3:6" s="31" customFormat="1"/>
-    <row r="59" spans="3:6" s="31" customFormat="1">
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="34"/>
-    </row>
+    <row r="59" spans="3:6" s="31" customFormat="1"/>
     <row r="60" spans="3:6" s="31" customFormat="1"/>
     <row r="61" spans="3:6" s="31" customFormat="1"/>
     <row r="62" spans="3:6" s="31" customFormat="1"/>
     <row r="63" spans="3:6" s="31" customFormat="1"/>
     <row r="64" spans="3:6" s="31" customFormat="1"/>
-    <row r="65" spans="3:6" s="31" customFormat="1"/>
+    <row r="65" spans="3:6" s="31" customFormat="1">
+      <c r="C65" s="59"/>
+      <c r="D65" s="59"/>
+      <c r="E65" s="59"/>
+      <c r="F65" s="59"/>
+    </row>
     <row r="66" spans="3:6" s="31" customFormat="1"/>
     <row r="67" spans="3:6" s="31" customFormat="1">
-      <c r="C67" s="59"/>
-      <c r="D67" s="59"/>
-      <c r="E67" s="59"/>
-      <c r="F67" s="59"/>
+      <c r="D67" s="34"/>
+      <c r="E67" s="34"/>
+      <c r="F67" s="34"/>
     </row>
     <row r="68" spans="3:6" s="31" customFormat="1"/>
-    <row r="69" spans="3:6" s="31" customFormat="1">
-      <c r="D69" s="34"/>
-      <c r="E69" s="34"/>
-      <c r="F69" s="34"/>
-    </row>
+    <row r="69" spans="3:6" s="31" customFormat="1"/>
     <row r="70" spans="3:6" s="31" customFormat="1"/>
     <row r="71" spans="3:6" s="31" customFormat="1"/>
     <row r="72" spans="3:6" s="31" customFormat="1"/>
@@ -40857,20 +41792,20 @@
     <row r="85" spans="3:6" s="31" customFormat="1"/>
     <row r="86" spans="3:6" s="31" customFormat="1"/>
     <row r="87" spans="3:6" s="31" customFormat="1"/>
-    <row r="88" spans="3:6" s="31" customFormat="1"/>
+    <row r="88" spans="3:6" s="31" customFormat="1">
+      <c r="C88" s="59"/>
+      <c r="D88" s="59"/>
+      <c r="E88" s="59"/>
+      <c r="F88" s="59"/>
+    </row>
     <row r="89" spans="3:6" s="31" customFormat="1"/>
     <row r="90" spans="3:6" s="31" customFormat="1">
-      <c r="C90" s="59"/>
-      <c r="D90" s="59"/>
-      <c r="E90" s="59"/>
-      <c r="F90" s="59"/>
+      <c r="D90" s="34"/>
+      <c r="E90" s="34"/>
+      <c r="F90" s="34"/>
     </row>
     <row r="91" spans="3:6" s="31" customFormat="1"/>
-    <row r="92" spans="3:6" s="31" customFormat="1">
-      <c r="D92" s="34"/>
-      <c r="E92" s="34"/>
-      <c r="F92" s="34"/>
-    </row>
+    <row r="92" spans="3:6" s="31" customFormat="1"/>
     <row r="93" spans="3:6" s="31" customFormat="1"/>
     <row r="94" spans="3:6" s="31" customFormat="1"/>
     <row r="95" spans="3:6" s="31" customFormat="1"/>
@@ -40878,20 +41813,20 @@
     <row r="97" spans="3:6" s="31" customFormat="1"/>
     <row r="98" spans="3:6" s="31" customFormat="1"/>
     <row r="99" spans="3:6" s="31" customFormat="1"/>
-    <row r="100" spans="3:6" s="31" customFormat="1"/>
+    <row r="100" spans="3:6" s="31" customFormat="1">
+      <c r="C100" s="59"/>
+      <c r="D100" s="59"/>
+      <c r="E100" s="59"/>
+      <c r="F100" s="59"/>
+    </row>
     <row r="101" spans="3:6" s="31" customFormat="1"/>
     <row r="102" spans="3:6" s="31" customFormat="1">
-      <c r="C102" s="59"/>
-      <c r="D102" s="59"/>
-      <c r="E102" s="59"/>
-      <c r="F102" s="59"/>
+      <c r="D102" s="34"/>
+      <c r="E102" s="34"/>
+      <c r="F102" s="34"/>
     </row>
     <row r="103" spans="3:6" s="31" customFormat="1"/>
-    <row r="104" spans="3:6" s="31" customFormat="1">
-      <c r="D104" s="34"/>
-      <c r="E104" s="34"/>
-      <c r="F104" s="34"/>
-    </row>
+    <row r="104" spans="3:6" s="31" customFormat="1"/>
     <row r="105" spans="3:6" s="31" customFormat="1"/>
     <row r="106" spans="3:6" s="31" customFormat="1"/>
     <row r="107" spans="3:6" s="31" customFormat="1"/>
@@ -40903,20 +41838,20 @@
     <row r="113" spans="3:6" s="31" customFormat="1"/>
     <row r="114" spans="3:6" s="31" customFormat="1"/>
     <row r="115" spans="3:6" s="31" customFormat="1"/>
-    <row r="116" spans="3:6" s="31" customFormat="1"/>
+    <row r="116" spans="3:6" s="31" customFormat="1">
+      <c r="C116" s="59"/>
+      <c r="D116" s="59"/>
+      <c r="E116" s="59"/>
+      <c r="F116" s="59"/>
+    </row>
     <row r="117" spans="3:6" s="31" customFormat="1"/>
     <row r="118" spans="3:6" s="31" customFormat="1">
-      <c r="C118" s="59"/>
-      <c r="D118" s="59"/>
-      <c r="E118" s="59"/>
-      <c r="F118" s="59"/>
+      <c r="D118" s="34"/>
+      <c r="E118" s="34"/>
+      <c r="F118" s="34"/>
     </row>
     <row r="119" spans="3:6" s="31" customFormat="1"/>
-    <row r="120" spans="3:6" s="31" customFormat="1">
-      <c r="D120" s="34"/>
-      <c r="E120" s="34"/>
-      <c r="F120" s="34"/>
-    </row>
+    <row r="120" spans="3:6" s="31" customFormat="1"/>
     <row r="121" spans="3:6" s="31" customFormat="1"/>
     <row r="122" spans="3:6" s="31" customFormat="1"/>
     <row r="123" spans="3:6" s="31" customFormat="1"/>
@@ -41008,25 +41943,23 @@
     <row r="209" s="31" customFormat="1"/>
     <row r="210" s="31" customFormat="1"/>
     <row r="211" s="31" customFormat="1"/>
-    <row r="212" s="31" customFormat="1"/>
-    <row r="213" s="31" customFormat="1"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C90:F90"/>
-    <mergeCell ref="C102:F102"/>
-    <mergeCell ref="C118:F118"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C67:F67"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="B4:C4"/>
+    <mergeCell ref="C88:F88"/>
+    <mergeCell ref="C100:F100"/>
+    <mergeCell ref="C116:F116"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="C55:F55"/>
+    <mergeCell ref="C65:F65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -41038,7 +41971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H30"/>
   <sheetViews>
-    <sheetView zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -41057,7 +41990,7 @@
   <sheetData>
     <row r="3" spans="2:8" ht="15.6" customHeight="1">
       <c r="B3" s="67" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C3" s="67"/>
       <c r="D3" s="67"/>
@@ -41077,25 +42010,25 @@
     </row>
     <row r="5" spans="2:8" ht="30">
       <c r="B5" s="41" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G5" s="41" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H5" s="41" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="30">
@@ -41103,20 +42036,20 @@
         <v>1</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="H6" s="44" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="30">
@@ -41124,20 +42057,20 @@
         <v>2</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="H7" s="44" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="2:8">

</xml_diff>